<commit_message>
Knudsen model for boron coatings
</commit_message>
<xml_diff>
--- a/data_processing/2025/optical density/data/Optical transmission measurements.xlsx
+++ b/data_processing/2025/optical density/data/Optical transmission measurements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickmartinez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erickmartinez/Library/Mobile Documents/com~apple~CloudDocs/Documents/GitHub/relozwall/data_processing/2025/optical density/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186A64EA-C272-D84D-A17E-CDC19F2D9952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC07716-B0AA-2B45-834D-94D1787C4C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deposition cone" sheetId="2" r:id="rId1"/>
@@ -126,30 +126,35 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -11409,7 +11414,9 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>